<commit_message>
vitrine routes related stuff
</commit_message>
<xml_diff>
--- a/documents/api_routes.xlsx
+++ b/documents/api_routes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="85">
   <si>
     <t xml:space="preserve">Status</t>
   </si>
@@ -134,9 +134,6 @@
   </si>
   <si>
     <t xml:space="preserve">Vitrine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TODO</t>
   </si>
   <si>
     <t xml:space="preserve">/vitrines</t>
@@ -157,6 +154,9 @@
     <t xml:space="preserve">Create new vitrine</t>
   </si>
   <si>
+    <t xml:space="preserve">TODO</t>
+  </si>
+  <si>
     <t xml:space="preserve">/vitrines/:latitude/:longitude</t>
   </si>
   <si>
@@ -164,6 +164,16 @@
   </si>
   <si>
     <t xml:space="preserve">Get vitrines close to a position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAYBE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list of vitrines containing the 
+Position wihthin their radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get vitrines you can post to</t>
   </si>
   <si>
     <t xml:space="preserve">/vitrines/:vitrineId</t>
@@ -212,7 +222,10 @@
     <t xml:space="preserve">/pictures</t>
   </si>
   <si>
-    <t xml:space="preserve">vitrineId</t>
+    <t xml:space="preserve">VitrineId
+Latitude
+Longitude
+Multipart : File</t>
   </si>
   <si>
     <t xml:space="preserve">Created picture in json</t>
@@ -323,7 +336,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -340,6 +353,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCE181E"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF95C5F9"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -391,7 +416,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -424,6 +449,14 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -437,7 +470,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCE181E"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -471,7 +504,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FF95C5F9"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -501,12 +534,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -748,11 +781,11 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>16</v>
@@ -765,15 +798,15 @@
         <v>29</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>10</v>
@@ -782,18 +815,18 @@
         <v>21</v>
       </c>
       <c r="E16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="4" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>43</v>
@@ -812,52 +845,50 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+    <row r="18" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="F18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="A19" s="4"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
         <v>50</v>
       </c>
@@ -865,205 +896,207 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
-        <v>37</v>
+    <row r="21" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="F21" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
+      <c r="A22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="A23" s="4"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="G25" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
+      <c r="E28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="A29" s="4"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="G30" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
+      <c r="C31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="A32" s="4"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>71</v>
@@ -1084,87 +1117,108 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="G34" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
+      <c r="C35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="5" t="s">
+      <c r="F35" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G35" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F37" s="4" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>81</v>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1178,8 +1232,8 @@
     <mergeCell ref="F3:F5"/>
     <mergeCell ref="G3:G5"/>
     <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A37:G37"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>